<commit_message>
atualização no módulo vigência contratos
</commit_message>
<xml_diff>
--- a/database/controle_pregoeiros.xlsx
+++ b/database/controle_pregoeiros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/63fbdbda17b5124d/Área de Trabalho/PyQt6/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb5bd7a50d11ebd7/Área de Trabalho/pyqt6/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{D3E435E0-CC35-4EB2-9E45-2D1C21F6A914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64A3C671-3915-439B-AB0F-80F60B203EB0}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{D3E435E0-CC35-4EB2-9E45-2D1C21F6A914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65C7F27F-3985-4028-8D69-B49D0BBAB769}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{341CBEDB-42CC-489D-8461-7CAB6C7C262D}"/>
+    <workbookView xWindow="12470" yWindow="5370" windowWidth="28800" windowHeight="15460" xr2:uid="{341CBEDB-42CC-489D-8461-7CAB6C7C262D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>nome</t>
   </si>
@@ -44,40 +44,34 @@
     <t>antiguidade</t>
   </si>
   <si>
-    <t>Bruno</t>
-  </si>
-  <si>
-    <t>Rodolfo</t>
-  </si>
-  <si>
-    <t>Rodrigo</t>
-  </si>
-  <si>
-    <t>Guilherme</t>
-  </si>
-  <si>
-    <t>Laia</t>
-  </si>
-  <si>
-    <t>Creni</t>
-  </si>
-  <si>
-    <t>Messias</t>
-  </si>
-  <si>
-    <t>Mendonça</t>
-  </si>
-  <si>
-    <t>Lucheti</t>
-  </si>
-  <si>
-    <t>Andressa</t>
-  </si>
-  <si>
-    <t>Vicente</t>
-  </si>
-  <si>
-    <t>Ivanilda</t>
+    <t>Ten Juliana Araújo</t>
+  </si>
+  <si>
+    <t>Ten Shayane</t>
+  </si>
+  <si>
+    <t>Ten Ana Paula</t>
+  </si>
+  <si>
+    <t>SO Lôbo</t>
+  </si>
+  <si>
+    <t>1ºSG Vasconcelos</t>
+  </si>
+  <si>
+    <t>2ºSG Macário</t>
+  </si>
+  <si>
+    <t>3ºSG Beatriz</t>
+  </si>
+  <si>
+    <t>3ºSG Dimas</t>
+  </si>
+  <si>
+    <t>3ºSG Petterson</t>
+  </si>
+  <si>
+    <t>3ºSG Joan</t>
   </si>
 </sst>
 </file>
@@ -136,9 +130,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -176,7 +170,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -282,7 +276,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -424,7 +418,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -432,18 +426,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADCB3E7-5383-4BAF-AFD0-88522CB3AD5D}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="1" max="1" width="24.26953125" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,7 +446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -459,7 +454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -467,7 +462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -475,7 +470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -483,7 +478,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -491,7 +486,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -499,7 +494,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -507,7 +502,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -515,7 +510,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -523,28 +518,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>